<commit_message>
cosmetic fix - removed spaces
</commit_message>
<xml_diff>
--- a/medico-triage-backend/Symptom-Diagnosis-Linear-matrix.xlsx
+++ b/medico-triage-backend/Symptom-Diagnosis-Linear-matrix.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ac046137/Sites/Python Projects/DiagnosisPrediction/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ac046137/Sites/Python Projects/Innovation_challenge_4_OracleCerner_Final_submission/medico-triage-backend/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0EA7903-5C94-2444-8814-A50F15788B57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B01F6A8B-7582-9140-9F1D-1CCBFA236F1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{44E48FA9-23A4-F848-9899-B2CF7E423537}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19560" xr2:uid="{44E48FA9-23A4-F848-9899-B2CF7E423537}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -178,9 +178,6 @@
     <t>Cerebrovascular Accident (Stroke)</t>
   </si>
   <si>
-    <t xml:space="preserve"> Common cold/Influenza</t>
-  </si>
-  <si>
     <t>Diarrhea</t>
   </si>
   <si>
@@ -215,6 +212,9 @@
   </si>
   <si>
     <t>Cirrhosis of Liver</t>
+  </si>
+  <si>
+    <t>Common cold/Influenza</t>
   </si>
 </sst>
 </file>
@@ -581,7 +581,7 @@
   <dimension ref="A1:AT85"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1175,7 +1175,7 @@
     </row>
     <row r="5" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="B5" s="3">
         <v>1</v>
@@ -1312,7 +1312,7 @@
     </row>
     <row r="6" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B6" s="3">
         <v>1</v>
@@ -1449,7 +1449,7 @@
     </row>
     <row r="7" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B7" s="3">
         <v>1</v>
@@ -1586,7 +1586,7 @@
     </row>
     <row r="8" spans="1:46" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B8" s="3">
         <v>0</v>
@@ -1723,7 +1723,7 @@
     </row>
     <row r="9" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B9" s="3">
         <v>0</v>
@@ -1860,7 +1860,7 @@
     </row>
     <row r="10" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B10" s="3">
         <v>0</v>
@@ -1997,7 +1997,7 @@
     </row>
     <row r="11" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B11" s="3">
         <v>0</v>
@@ -2134,7 +2134,7 @@
     </row>
     <row r="12" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B12" s="3">
         <v>0</v>
@@ -2271,7 +2271,7 @@
     </row>
     <row r="13" spans="1:46" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B13" s="3">
         <v>1</v>
@@ -2408,7 +2408,7 @@
     </row>
     <row r="14" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B14" s="3">
         <v>0</v>
@@ -2545,7 +2545,7 @@
     </row>
     <row r="15" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B15" s="3">
         <v>1</v>
@@ -2682,7 +2682,7 @@
     </row>
     <row r="16" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B16" s="3">
         <v>0</v>
@@ -2819,7 +2819,7 @@
     </row>
     <row r="17" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B17" s="3">
         <v>0</v>

</xml_diff>